<commit_message>
hinzufuegen Risiko Allgemein und Aktualisierung Projektplan
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09762C71-CEA9-7246-BE31-F795F0548DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD91635-D413-A947-B75F-BA5C6E28878D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -80,27 +80,15 @@
     <t>Problemanalyse</t>
   </si>
   <si>
-    <t>Stakeholderanalyse</t>
-  </si>
-  <si>
     <t>Erfordernisse</t>
   </si>
   <si>
     <t>Anforderungen</t>
   </si>
   <si>
-    <t>User Profiles</t>
-  </si>
-  <si>
-    <t>Personas</t>
-  </si>
-  <si>
     <t>Problemszenario</t>
   </si>
   <si>
-    <t>How-Might-We?</t>
-  </si>
-  <si>
     <t>Kommunikationsmodell</t>
   </si>
   <si>
@@ -128,15 +116,9 @@
     <t>Bug fixes</t>
   </si>
   <si>
-    <t>Lösungsfindung: warum eine Webseite/App?</t>
-  </si>
-  <si>
     <t>Folien 3 Audit</t>
   </si>
   <si>
-    <t>Folien 2 Audit</t>
-  </si>
-  <si>
     <t>Time-Tracking</t>
   </si>
   <si>
@@ -158,9 +140,6 @@
     <t>Folien 1 Audit</t>
   </si>
   <si>
-    <t>PoCs</t>
-  </si>
-  <si>
     <t>09.12.22 (Abgabe auf GitHub)</t>
   </si>
   <si>
@@ -185,12 +164,6 @@
     <t>24.02.22(Abgabe auf GitHub)</t>
   </si>
   <si>
-    <t>Projektrisiken allgemein</t>
-  </si>
-  <si>
-    <t>Spezifikation der Fail-Kriterien, Fallbacks</t>
-  </si>
-  <si>
     <t>15min</t>
   </si>
   <si>
@@ -219,6 +192,36 @@
   </si>
   <si>
     <t xml:space="preserve">Niedrig </t>
+  </si>
+  <si>
+    <t>Steakholderanalyse</t>
+  </si>
+  <si>
+    <t>Lösungsfindung: warum eine Webseite/App? (Repository)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
+    <t>Spezifikation der Fail-Kriterien, Fallbacks (Begründen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoCs definieren </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folien 2 Audit (PP-Folien, Kommentierte Datei) </t>
+  </si>
+  <si>
+    <t>Projektrisiken Konsequenzen und Maßnahmen (Allgemein)</t>
+  </si>
+  <si>
+    <t>Projektrisiken im allgemeinen (Allgemein)</t>
+  </si>
+  <si>
+    <t>Projektrisiken Kosnequenzen und Maßnahmen (Projektbezogen)</t>
+  </si>
+  <si>
+    <t>3h</t>
   </si>
 </sst>
 </file>
@@ -288,12 +291,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +302,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -483,7 +487,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -498,18 +502,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,62 +524,61 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -594,15 +588,17 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -635,138 +631,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -821,6 +685,43 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -831,6 +732,99 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -980,18 +974,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B4:J28" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B4:J28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B4:J35" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B4:J35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Alba" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{017F0763-4A73-A643-AF78-71BC291F7337}" name="Time-Tracking" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Losik" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{961BA321-F622-CC4F-8731-C958ED4A26FD}" name="Time-Tracking2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6C75E308-AC3B-A24C-A8BD-6318A29D4398}" name="Beni" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Alba" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{017F0763-4A73-A643-AF78-71BC291F7337}" name="Time-Tracking" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Losik" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{961BA321-F622-CC4F-8731-C958ED4A26FD}" name="Time-Tracking2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6C75E308-AC3B-A24C-A8BD-6318A29D4398}" name="Beni" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{528EF0AD-B051-4F49-B985-D81C998E0E25}" name="Time-Tracking3" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorität " dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorität " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,89 +1288,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:L39"/>
+  <dimension ref="B3:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="53" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="46" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="B3" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="34">
+      <c r="B5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="28">
         <v>44859</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="50"/>
+        <v>38</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="20" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1384,29 +1378,29 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="29">
         <v>44864</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>10</v>
@@ -1414,23 +1408,23 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="35">
+        <v>28</v>
+      </c>
+      <c r="C7" s="29">
         <v>44865</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>55</v>
+        <v>38</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="46"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="46"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>9</v>
@@ -1438,23 +1432,23 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="35">
+        <v>36</v>
+      </c>
+      <c r="C8" s="29">
         <v>44867</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="46"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="46"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>11</v>
@@ -1462,405 +1456,533 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="35">
+        <v>37</v>
+      </c>
+      <c r="C9" s="29">
         <v>44869</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="38"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="46"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="46" t="s">
-        <v>54</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="35">
+      <c r="B10" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="29">
         <v>44874</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="46"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="6" t="s">
-        <v>60</v>
+      <c r="B12" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="29">
+        <v>44883</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="48"/>
+        <v>58</v>
+      </c>
+      <c r="C14" s="29">
+        <v>44885</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="48"/>
+        <v>60</v>
+      </c>
+      <c r="C15" s="29">
+        <v>44886</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="C16" s="29">
+        <v>44889</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="41"/>
+      <c r="J16" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="4" t="s">
-        <v>59</v>
+      <c r="B17" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="29">
+        <v>44889</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="4" t="s">
-        <v>59</v>
+      <c r="B18" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="29">
+        <v>44889</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="5" t="s">
-        <v>58</v>
+      <c r="B19" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="29">
+        <v>44893</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="C20" s="29">
+        <v>44893</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="41"/>
+      <c r="J20" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="13"/>
-      <c r="L21" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C21" s="29">
+        <v>44893</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="41"/>
+      <c r="H21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="41"/>
+      <c r="J21" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="18"/>
+      <c r="B22" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="29">
+        <v>44900</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="41"/>
+      <c r="H22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="41"/>
+      <c r="J22" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="13"/>
+      <c r="B23" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="29">
+        <v>44900</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="41"/>
+      <c r="H23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="41"/>
+      <c r="J23" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="13"/>
+      <c r="B24" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="29">
+        <v>44900</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="C25" s="29">
+        <v>44904</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="18"/>
+      <c r="B26" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="40"/>
+      <c r="H26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="40"/>
+      <c r="J26" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="12"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+      <c r="C34" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="21"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="55"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="55"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="55"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="55"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="55"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="56"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="55"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C40"/>
+      <c r="E40"/>
+      <c r="G40"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C41"/>
+      <c r="E41"/>
+      <c r="G41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C42"/>
+      <c r="E42"/>
+      <c r="G42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C43"/>
+      <c r="E43"/>
+      <c r="G43"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C44"/>
+      <c r="E44"/>
+      <c r="G44"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C45"/>
+      <c r="E45"/>
+      <c r="G45"/>
+      <c r="I45"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Hinzufuegen neuer Dateien und Aktualisierung des Projektplans
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898FCB55-817F-6446-86BA-EA2EBAB0C615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92053F5D-92C8-6D4F-A994-71EBBC019B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="920" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="81">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Domänenmodell Soll-Zustand Version 2.0  (unser System)</t>
   </si>
   <si>
-    <t>Kommunikationsdiagramm</t>
-  </si>
-  <si>
     <t>Datenstruktur</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
   </si>
   <si>
     <t>Sequenzdiagramm</t>
-  </si>
-  <si>
-    <t>Evulation</t>
   </si>
   <si>
     <r>
@@ -288,9 +282,6 @@
     <t>Wiki im Repository auf dem Laufenden halten</t>
   </si>
   <si>
-    <t>Code (mit Kommentaren)</t>
-  </si>
-  <si>
     <t>Folien 1 Audit Hochladen</t>
   </si>
   <si>
@@ -301,6 +292,15 @@
   </si>
   <si>
     <t>Time-Tracking1</t>
+  </si>
+  <si>
+    <t>Erste Code-Entwürfe (mit Kommentaren)</t>
+  </si>
+  <si>
+    <t>Kommunikationsdiagramm/HTA</t>
+  </si>
+  <si>
+    <t>Evulation/ Betrachtung und Bewertung Alternativen</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -578,6 +578,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,7 +596,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -696,9 +707,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -748,6 +756,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -758,15 +772,8 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -774,8 +781,12 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -998,24 +1009,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -1057,6 +1050,27 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1146,11 +1160,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B3:J56" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B3:J56" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B3:J56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Alba" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{017F0763-4A73-A643-AF78-71BC291F7337}" name="Time-Tracking1" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Losik" dataDxfId="5"/>
@@ -1462,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1476,52 +1490,52 @@
     <col min="7" max="7" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="44"/>
     <col min="9" max="9" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="67" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="66" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="72" t="s">
+      <c r="E3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="74" t="s">
+      <c r="J3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="68" t="s">
+      <c r="L3" s="67" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1542,7 +1556,7 @@
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="26"/>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="58" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1574,7 +1588,7 @@
       <c r="I5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="58" t="s">
         <v>39</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -1598,7 +1612,7 @@
       <c r="G6" s="28"/>
       <c r="H6" s="29"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="58" t="s">
         <v>39</v>
       </c>
       <c r="L6" s="6" t="s">
@@ -1622,17 +1636,17 @@
       <c r="G7" s="28"/>
       <c r="H7" s="29"/>
       <c r="I7" s="28"/>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="59" t="s">
         <v>40</v>
       </c>
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="46" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>55</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="27"/>
@@ -1644,7 +1658,7 @@
       <c r="I8" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1665,13 +1679,13 @@
       <c r="I9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="58" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="57" t="s">
-        <v>77</v>
+      <c r="B10" s="56" t="s">
+        <v>74</v>
       </c>
       <c r="C10" s="46" t="s">
         <v>26</v>
@@ -1690,7 +1704,7 @@
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1711,7 +1725,7 @@
       <c r="I11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1719,39 +1733,45 @@
       <c r="B12" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="46">
         <v>44889</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="30" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="23"/>
       <c r="G12" s="32"/>
       <c r="H12" s="23"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="58" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="20">
+        <v>62</v>
+      </c>
+      <c r="C13" s="46">
         <v>44889</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="30" t="s">
+        <v>69</v>
+      </c>
       <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="32" t="s">
+        <v>69</v>
+      </c>
       <c r="H13" s="23"/>
       <c r="I13" s="32"/>
-      <c r="J13" s="60" t="s">
+      <c r="J13" s="59" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1770,13 +1790,13 @@
       <c r="G14" s="32"/>
       <c r="H14" s="33"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="60" t="s">
+      <c r="J14" s="59" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" s="20">
         <v>44889</v>
@@ -1791,13 +1811,13 @@
       <c r="G15" s="32"/>
       <c r="H15" s="23"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="59" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C16" s="20">
         <v>44889</v>
@@ -1805,18 +1825,18 @@
       <c r="D16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="61" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C17" s="20">
         <v>44889</v>
@@ -1829,167 +1849,175 @@
       <c r="G17" s="32"/>
       <c r="H17" s="23"/>
       <c r="I17" s="32"/>
-      <c r="J17" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="20">
+      <c r="J17" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="46">
+        <v>44893</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="20">
         <v>44889</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="46">
-        <v>44893</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="F19" s="23"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="46">
+        <v>44883</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="20">
-        <v>44893</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="47" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C21" s="46">
-        <v>44883</v>
+        <v>44885</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F21" s="31"/>
       <c r="G21" s="32"/>
       <c r="H21" s="33"/>
       <c r="I21" s="32"/>
-      <c r="J21" s="60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="47" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="46">
-        <v>44885</v>
-      </c>
-      <c r="D22" s="7" t="s">
+        <v>44886</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="32"/>
-      <c r="J22" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="46">
-        <v>44886</v>
+        <v>44899</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="47" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C24" s="46">
         <v>44899</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>70</v>
-      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="23" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="H24" s="23" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="J24" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="J24" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="46">
-        <v>44899</v>
+        <v>78</v>
+      </c>
+      <c r="C25" s="20">
+        <v>44902</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="30"/>
@@ -1997,257 +2025,245 @@
         <v>28</v>
       </c>
       <c r="G25" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="20">
+        <v>44902</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="51"/>
+      <c r="F26" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="52"/>
+      <c r="H26" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="52"/>
+      <c r="J26" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="20">
+        <v>44902</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="51"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="20">
+        <v>44904</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="32"/>
+      <c r="J28" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20">
+        <v>44904</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="32"/>
+      <c r="J29" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="20">
+        <v>44904</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="30"/>
+      <c r="F31" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="36"/>
+      <c r="H31" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="36"/>
+      <c r="J31" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="54"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="54"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J25" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="46">
-        <v>44899</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="46">
-        <v>44899</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="20">
-        <v>44899</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28" s="32"/>
-      <c r="J28" s="60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="20">
-        <v>44902</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="J29" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="20">
-        <v>44902</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="51"/>
-      <c r="F30" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="52"/>
-      <c r="H30" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="52"/>
-      <c r="J30" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="20">
-        <v>44902</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="51"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="20">
-        <v>44904</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="20">
-        <v>44904</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="32"/>
-      <c r="J33" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="20">
-        <v>44904</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="32"/>
       <c r="H34" s="23"/>
       <c r="I34" s="32"/>
       <c r="J34" s="59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="54"/>
+      <c r="D35" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="30"/>
       <c r="F35" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="36"/>
+      <c r="G35" s="32"/>
       <c r="H35" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="36"/>
+      <c r="I35" s="32"/>
       <c r="J35" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="14"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="9"/>
       <c r="E36" s="30"/>
       <c r="F36" s="31"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="32"/>
-      <c r="J36" s="62"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J36" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>15</v>
       </c>
@@ -2258,9 +2274,11 @@
       <c r="G37" s="36"/>
       <c r="H37" s="37"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="63"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J37" s="59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
@@ -2271,9 +2289,11 @@
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
       <c r="I38" s="32"/>
-      <c r="J38" s="64"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J38" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>17</v>
       </c>
@@ -2284,11 +2304,13 @@
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
       <c r="I39" s="32"/>
-      <c r="J39" s="64"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J39" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="47" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C40" s="54"/>
       <c r="D40" s="9"/>
@@ -2297,11 +2319,13 @@
       <c r="G40" s="32"/>
       <c r="H40" s="23"/>
       <c r="I40" s="32"/>
-      <c r="J40" s="65"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J40" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="55" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C41" s="54"/>
       <c r="D41" s="8"/>
@@ -2310,11 +2334,11 @@
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
       <c r="I41" s="32"/>
-      <c r="J41" s="64"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J41" s="75"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="7"/>
@@ -2323,11 +2347,11 @@
       <c r="G42" s="52"/>
       <c r="H42" s="23"/>
       <c r="I42" s="52"/>
-      <c r="J42" s="65"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J42" s="64"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C43" s="54"/>
       <c r="D43" s="7"/>
@@ -2336,11 +2360,11 @@
       <c r="G43" s="52"/>
       <c r="H43" s="23"/>
       <c r="I43" s="52"/>
-      <c r="J43" s="65"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J43" s="64"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="54"/>
       <c r="D44" s="7"/>
@@ -2349,11 +2373,11 @@
       <c r="G44" s="32"/>
       <c r="H44" s="7"/>
       <c r="I44" s="32"/>
-      <c r="J44" s="65"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J44" s="64"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="54"/>
       <c r="D45" s="7"/>
@@ -2362,11 +2386,11 @@
       <c r="G45" s="32"/>
       <c r="H45" s="7"/>
       <c r="I45" s="32"/>
-      <c r="J45" s="65"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J45" s="64"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="54"/>
       <c r="D46" s="7"/>
@@ -2375,11 +2399,11 @@
       <c r="G46" s="32"/>
       <c r="H46" s="23"/>
       <c r="I46" s="32"/>
-      <c r="J46" s="65"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B47" s="58" t="s">
-        <v>78</v>
+      <c r="J46" s="64"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>30</v>
@@ -2390,9 +2414,9 @@
       <c r="G47" s="32"/>
       <c r="H47" s="33"/>
       <c r="I47" s="32"/>
-      <c r="J47" s="63"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J47" s="62"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
@@ -2403,7 +2427,7 @@
       <c r="G48" s="32"/>
       <c r="H48" s="33"/>
       <c r="I48" s="32"/>
-      <c r="J48" s="62"/>
+      <c r="J48" s="61"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
@@ -2416,11 +2440,11 @@
       <c r="G49" s="36"/>
       <c r="H49" s="37"/>
       <c r="I49" s="36"/>
-      <c r="J49" s="64"/>
+      <c r="J49" s="63"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="9"/>
@@ -2429,11 +2453,11 @@
       <c r="G50" s="36"/>
       <c r="H50" s="37"/>
       <c r="I50" s="36"/>
-      <c r="J50" s="64"/>
+      <c r="J50" s="63"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="9"/>
@@ -2442,11 +2466,11 @@
       <c r="G51" s="36"/>
       <c r="H51" s="37"/>
       <c r="I51" s="36"/>
-      <c r="J51" s="64"/>
+      <c r="J51" s="63"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="9"/>
@@ -2455,11 +2479,11 @@
       <c r="G52" s="36"/>
       <c r="H52" s="37"/>
       <c r="I52" s="36"/>
-      <c r="J52" s="64"/>
+      <c r="J52" s="63"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="9"/>
@@ -2468,11 +2492,11 @@
       <c r="G53" s="36"/>
       <c r="H53" s="37"/>
       <c r="I53" s="36"/>
-      <c r="J53" s="64"/>
+      <c r="J53" s="63"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="9"/>
@@ -2481,11 +2505,11 @@
       <c r="G54" s="36"/>
       <c r="H54" s="37"/>
       <c r="I54" s="36"/>
-      <c r="J54" s="64"/>
+      <c r="J54" s="63"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="58" t="s">
-        <v>79</v>
+      <c r="B55" s="57" t="s">
+        <v>76</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>31</v>
@@ -2496,7 +2520,7 @@
       <c r="G55" s="32"/>
       <c r="H55" s="33"/>
       <c r="I55" s="32"/>
-      <c r="J55" s="62"/>
+      <c r="J55" s="61"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
@@ -2509,7 +2533,7 @@
       <c r="G56" s="41"/>
       <c r="H56" s="42"/>
       <c r="I56" s="41"/>
-      <c r="J56" s="66"/>
+      <c r="J56" s="65"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="19" t="s">
@@ -2523,7 +2547,7 @@
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C60"/>
       <c r="E60" s="44"/>

</xml_diff>

<commit_message>
Hinzufuegen Artefakte und Audit 2
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92053F5D-92C8-6D4F-A994-71EBBC019B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B733486F-883F-0E48-8A7B-81627E64FAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="80">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>Personas</t>
-  </si>
-  <si>
-    <t>W-Fragen (how might we?)</t>
   </si>
   <si>
     <t xml:space="preserve">Lösungsfindung: warum eine Webseite/App? </t>
@@ -459,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -578,17 +575,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -596,27 +582,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -632,58 +618,44 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -691,46 +663,39 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -745,13 +710,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,9 +721,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -771,24 +730,6 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -993,6 +934,24 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1160,18 +1119,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B3:J56" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B3:J56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="B3:J55" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="B3:J55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Alba" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{017F0763-4A73-A643-AF78-71BC291F7337}" name="Time-Tracking1" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Losik" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{961BA321-F622-CC4F-8731-C958ED4A26FD}" name="Time-Tracking2" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{6C75E308-AC3B-A24C-A8BD-6318A29D4398}" name="Beni" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{528EF0AD-B051-4F49-B985-D81C998E0E25}" name="Time-Tracking3" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorität " dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Deadline" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Alba" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{017F0763-4A73-A643-AF78-71BC291F7337}" name="Time-Tracking1" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Losik" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{961BA321-F622-CC4F-8731-C958ED4A26FD}" name="Time-Tracking2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6C75E308-AC3B-A24C-A8BD-6318A29D4398}" name="Beni" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{528EF0AD-B051-4F49-B985-D81C998E0E25}" name="Time-Tracking3" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorität " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1474,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L63"/>
+  <dimension ref="B2:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1485,57 +1444,55 @@
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" style="16" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="44"/>
-    <col min="7" max="7" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="44"/>
-    <col min="9" max="9" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="57" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="71" t="s">
+      <c r="E3" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I3" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="67" t="s">
+      <c r="L3" s="58" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1543,20 +1500,20 @@
       <c r="B4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="39">
         <v>44859</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="24" t="s">
+      <c r="F4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="58" t="s">
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="50" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1567,28 +1524,28 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="40">
         <v>44864</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="28" t="s">
+      <c r="H5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="50" t="s">
         <v>39</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -1599,20 +1556,20 @@
       <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="40">
         <v>44865</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="58" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="50" t="s">
         <v>39</v>
       </c>
       <c r="L6" s="6" t="s">
@@ -1623,155 +1580,155 @@
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="40">
         <v>44867</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="59" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="51" t="s">
         <v>40</v>
       </c>
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="28" t="s">
+      <c r="E8" s="26"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="58" t="s">
+      <c r="J8" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="40">
         <v>44874</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="28" t="s">
+      <c r="E9" s="26"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="46" t="s">
+      <c r="B10" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="58" t="s">
+      <c r="H10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="40">
         <v>44889</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="28"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="40">
         <v>44889</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="58" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="40">
         <v>44889</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>69</v>
+      <c r="E13" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="59" t="s">
+      <c r="G13" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="51" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1785,261 +1742,273 @@
       <c r="D14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="59" t="s">
+      <c r="E14" s="29"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="51" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="20">
+      <c r="B15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="40">
         <v>44889</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="59" t="s">
-        <v>40</v>
+      <c r="E15" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="50" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="20">
+        <v>70</v>
+      </c>
+      <c r="C16" s="40">
         <v>44889</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="58" t="s">
+      <c r="E16" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="40">
+        <v>44893</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="40">
+        <v>44889</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="20">
-        <v>44889</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="46">
-        <v>44893</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="32" t="s">
+      <c r="C19" s="40">
+        <v>44883</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="40">
+        <v>44885</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="40">
+        <v>44886</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="40">
+        <v>44899</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="40">
+        <v>44899</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="H23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="40">
+        <v>44902</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="20">
-        <v>44889</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="47" t="s">
+      <c r="C25" s="40">
+        <v>44902</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="43" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="46">
-        <v>44883</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="46">
-        <v>44885</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="46">
-        <v>44886</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="46">
-        <v>44899</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="46">
-        <v>44899</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="20">
-        <v>44902</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="C26" s="20">
         <v>44902</v>
@@ -2047,64 +2016,68 @@
       <c r="D26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="52"/>
-      <c r="H26" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="52"/>
-      <c r="J26" s="58" t="s">
+      <c r="E26" s="44"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="20">
-        <v>44902</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="58" t="s">
+      <c r="B27" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="40">
+        <v>44904</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="20">
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="40">
         <v>44904</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="30"/>
+      <c r="E28" s="29" t="s">
+        <v>32</v>
+      </c>
       <c r="F28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28" s="32"/>
-      <c r="J28" s="58" t="s">
+      <c r="G28" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" s="20">
         <v>44904</v>
@@ -2112,466 +2085,499 @@
       <c r="D29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="32"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="30"/>
       <c r="H29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="32"/>
-      <c r="J29" s="58" t="s">
+      <c r="I29" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="J29" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="20">
-        <v>44904</v>
+      <c r="B30" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="23"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="G30" s="32"/>
-      <c r="H30" s="23"/>
+      <c r="H30" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="I30" s="32"/>
-      <c r="J30" s="58" t="s">
-        <v>39</v>
-      </c>
+      <c r="J30" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="B31" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="14"/>
       <c r="D31" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="36"/>
-      <c r="H31" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="36"/>
-      <c r="J31" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="1"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="50" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="58" t="s">
+      <c r="B32" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="58" t="s">
-        <v>39</v>
+      <c r="B33" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="51" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="59" t="s">
+      <c r="B34" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="30"/>
+      <c r="J34" s="51" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="59" t="s">
-        <v>40</v>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="50" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
+        <v>15</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="32"/>
-      <c r="J36" s="58" t="s">
-        <v>39</v>
+      <c r="J36" s="51" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37" s="14"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="59" t="s">
-        <v>40</v>
+      <c r="D37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="50" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C38" s="14"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="58" t="s">
+      <c r="D38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="30"/>
+      <c r="H38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="30"/>
+      <c r="J38" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>17</v>
+      <c r="B39" s="41" t="s">
+        <v>65</v>
       </c>
       <c r="C39" s="14"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="58" t="s">
+      <c r="D39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="30"/>
+      <c r="H39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="30"/>
+      <c r="J39" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="34"/>
+      <c r="F40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="30"/>
+      <c r="J40" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="44"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="75"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="64"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="44"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="50" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="54"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="64"/>
+      <c r="B43" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="30"/>
+      <c r="H43" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="30"/>
+      <c r="J43" s="50" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="30"/>
+      <c r="B44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="29"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="32"/>
+      <c r="G44" s="30"/>
       <c r="H44" s="7"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="64"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="50" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="29"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="32"/>
+      <c r="G45" s="30"/>
       <c r="H45" s="7"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="64"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="50" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="64"/>
+      <c r="B46" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="54"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="B47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="62"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="53"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="31"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="8"/>
       <c r="G48" s="32"/>
       <c r="H48" s="33"/>
       <c r="I48" s="32"/>
-      <c r="J48" s="61"/>
+      <c r="J48" s="55"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>19</v>
+      <c r="B49" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="63"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="55"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="53" t="s">
-        <v>65</v>
+      <c r="B50" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="63"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="55"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="50" t="s">
-        <v>67</v>
+      <c r="B51" s="46" t="s">
+        <v>55</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="63"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="55"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B52" s="53" t="s">
-        <v>55</v>
+      <c r="B52" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="9"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="63"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="55"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="9"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="63"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="55"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="14"/>
+      <c r="B54" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="D54" s="9"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="63"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="53"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="9"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="61"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="65"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="56"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="19" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="19" t="s">
-        <v>48</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C59"/>
+      <c r="E59"/>
+      <c r="G59"/>
+      <c r="I59"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="19" t="s">
-        <v>61</v>
-      </c>
       <c r="C60"/>
-      <c r="E60" s="44"/>
-      <c r="G60" s="44"/>
-      <c r="I60" s="44"/>
+      <c r="E60"/>
+      <c r="G60"/>
+      <c r="I60"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="42"/>
       <c r="C61"/>
-      <c r="E61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="I61" s="44"/>
+      <c r="E61"/>
+      <c r="G61"/>
+      <c r="I61"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="49"/>
       <c r="C62"/>
-      <c r="E62" s="44"/>
-      <c r="G62" s="44"/>
-      <c r="I62" s="44"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C63"/>
-      <c r="E63" s="44"/>
-      <c r="G63" s="44"/>
-      <c r="I63" s="44"/>
+      <c r="E62"/>
+      <c r="G62"/>
+      <c r="I62"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Hinzufuegen Artefakte & Slides Audit 3
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/Alba_EP_Local_Repository/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA19D6AB-3B25-2347-B7EC-BE95D790F8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2437D339-F21B-D34E-B1EB-32E513AFD0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="86">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -309,17 +309,20 @@
     <t>Fazit</t>
   </si>
   <si>
+    <t xml:space="preserve">1,5h </t>
+  </si>
+  <si>
     <r>
-      <t>Nachbesserung Artefakte Audit 2: User Profiles anlegen,</t>
+      <t>Nachbesserung Artefakte Audit 2: User Profiles anlegen</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Funktionale und Non-Funktionale Anforderungen überarbeiten</t>
+      <t>, Funktionale und Non-Funktionale Anforderungen überarbeiten</t>
     </r>
     <r>
       <rPr>
@@ -333,7 +336,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1,5h </t>
+    <t>2,5h</t>
   </si>
 </sst>
 </file>
@@ -760,19 +763,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1486,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1503,17 +1506,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
@@ -2139,7 +2142,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="29"/>
@@ -2173,22 +2176,26 @@
     </row>
     <row r="31" spans="2:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B31" s="62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C31" s="63"/>
       <c r="D31" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="61"/>
-      <c r="G31" s="67"/>
+      <c r="E31" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="66" t="s">
+        <v>67</v>
+      </c>
       <c r="H31" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="67" t="s">
-        <v>66</v>
+      <c r="I31" s="66" t="s">
+        <v>67</v>
       </c>
       <c r="J31" s="64" t="s">
         <v>39</v>
@@ -2203,8 +2210,8 @@
       <c r="D32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="68" t="s">
-        <v>67</v>
+      <c r="E32" s="67" t="s">
+        <v>34</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="26"/>
@@ -2212,7 +2219,7 @@
         <v>28</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="J32" s="46" t="s">
         <v>39</v>
@@ -2242,18 +2249,20 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="68" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="13"/>
-      <c r="D34" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="D34" s="7"/>
       <c r="E34" s="28"/>
       <c r="F34" s="9"/>
       <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="29"/>
+      <c r="H34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="J34" s="46" t="s">
         <v>39</v>
       </c>
@@ -2304,11 +2313,15 @@
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="F37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="29"/>
+      <c r="G37" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="H37" s="30"/>
       <c r="I37" s="29"/>
       <c r="J37" s="47" t="s">
@@ -2325,11 +2338,15 @@
       <c r="F38" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="29"/>
+      <c r="G38" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="H38" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I38" s="29"/>
+      <c r="I38" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="J38" s="46" t="s">
         <v>39</v>
       </c>
@@ -2342,7 +2359,9 @@
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="28" t="s">
+        <v>66</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="41"/>
       <c r="H39" s="7"/>
@@ -2376,15 +2395,21 @@
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="28"/>
+      <c r="E41" s="28" t="s">
+        <v>67</v>
+      </c>
       <c r="F41" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="29"/>
+      <c r="G41" s="29" t="s">
+        <v>34</v>
+      </c>
       <c r="H41" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="29"/>
+      <c r="I41" s="29" t="s">
+        <v>34</v>
+      </c>
       <c r="J41" s="46" t="s">
         <v>39</v>
       </c>
@@ -2397,7 +2422,9 @@
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="28"/>
+      <c r="E42" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="F42" s="7"/>
       <c r="G42" s="29"/>
       <c r="H42" s="7"/>
@@ -2414,7 +2441,9 @@
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="28"/>
+      <c r="E43" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="29"/>
       <c r="H43" s="7"/>

</xml_diff>

<commit_message>
Aktueller Projektplan und Client_Server_Modell
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/Alba_EP_Local_Repository/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2379DFC4-7960-B64B-B3AB-EBBCD5B0D13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A9EAEE-EFBA-464A-B95E-B9071E63441C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="560" windowWidth="25380" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t xml:space="preserve">Priorität </t>
   </si>
   <si>
-    <t xml:space="preserve">Poster  </t>
-  </si>
-  <si>
     <t>Alba</t>
   </si>
   <si>
@@ -302,15 +299,9 @@
     <t>Gesamt Aufwand in std</t>
   </si>
   <si>
-    <t xml:space="preserve">Skizzierung User Interface </t>
-  </si>
-  <si>
     <t xml:space="preserve">Design Fiction/ Future System (Figma) </t>
   </si>
   <si>
-    <t xml:space="preserve">User Interface Design (Figma) </t>
-  </si>
-  <si>
     <t>Bug fixes (+ Dokumentation)</t>
   </si>
   <si>
@@ -339,6 +330,15 @@
   </si>
   <si>
     <t>Stand 13.02.23</t>
+  </si>
+  <si>
+    <t>Skizzierung User Interface (Basic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Interface Design Projektumsetzung (Figma) </t>
+  </si>
+  <si>
+    <t>Poster  erstellen</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -682,7 +682,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -829,13 +828,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1550,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="96" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="96" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1559,1575 +1560,1575 @@
     <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" style="15" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="34" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="49" t="s">
+      <c r="I3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="J3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="35" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="24">
         <v>44859</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="50"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="59">
+        <v>24</v>
+      </c>
+      <c r="G4" s="58">
         <v>15</v>
       </c>
       <c r="H4" s="21"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="32" t="s">
-        <v>27</v>
+      <c r="I4" s="64"/>
+      <c r="J4" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="25">
         <v>44864</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="51">
+        <v>24</v>
+      </c>
+      <c r="E5" s="50">
         <v>420</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="60">
+        <v>24</v>
+      </c>
+      <c r="G5" s="59">
         <v>420</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="60">
+        <v>24</v>
+      </c>
+      <c r="I5" s="59">
         <v>420</v>
       </c>
-      <c r="J5" s="32" t="s">
-        <v>27</v>
+      <c r="J5" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="25">
         <v>44865</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="51">
+        <v>24</v>
+      </c>
+      <c r="E6" s="50">
         <v>180</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" s="60"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="22"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="32" t="s">
-        <v>27</v>
+      <c r="I6" s="59"/>
+      <c r="J6" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="25">
         <v>44867</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="51">
+        <v>24</v>
+      </c>
+      <c r="E7" s="50">
         <v>90</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="60"/>
+      <c r="G7" s="59"/>
       <c r="H7" s="22"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="33" t="s">
-        <v>28</v>
+      <c r="I7" s="59"/>
+      <c r="J7" s="32" t="s">
+        <v>27</v>
       </c>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="51"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="60"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="60">
+        <v>24</v>
+      </c>
+      <c r="I8" s="59">
         <v>90</v>
       </c>
-      <c r="J8" s="32" t="s">
-        <v>27</v>
+      <c r="J8" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="25">
         <v>44874</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="51"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="60">
+        <v>24</v>
+      </c>
+      <c r="G9" s="59">
         <v>120</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="60">
+        <v>24</v>
+      </c>
+      <c r="I9" s="59">
         <v>120</v>
       </c>
-      <c r="J9" s="32" t="s">
-        <v>27</v>
+      <c r="J9" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
-        <v>40</v>
+      <c r="B10" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="25">
         <v>44874</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="51">
+        <v>24</v>
+      </c>
+      <c r="E10" s="50">
         <v>180</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="60">
+        <v>24</v>
+      </c>
+      <c r="G10" s="59">
         <v>180</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="60">
+        <v>24</v>
+      </c>
+      <c r="I10" s="59">
         <v>180</v>
       </c>
-      <c r="J10" s="32"/>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="25">
         <v>44874</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="51">
+        <v>24</v>
+      </c>
+      <c r="E11" s="50">
         <v>60</v>
       </c>
       <c r="F11" s="22"/>
-      <c r="G11" s="60"/>
+      <c r="G11" s="59"/>
       <c r="H11" s="22"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="32"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
-        <v>53</v>
+      <c r="B12" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="51">
+        <v>24</v>
+      </c>
+      <c r="E12" s="50">
         <v>15</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="60"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="32" t="s">
-        <v>27</v>
+      <c r="I12" s="59"/>
+      <c r="J12" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" s="25">
         <v>44889</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="51"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="60"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="60">
+        <v>24</v>
+      </c>
+      <c r="I13" s="59">
         <v>60</v>
       </c>
-      <c r="J13" s="32" t="s">
-        <v>27</v>
+      <c r="J13" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="25">
         <v>44889</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="52">
+        <v>24</v>
+      </c>
+      <c r="E14" s="51">
         <v>180</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="61"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="32" t="s">
-        <v>27</v>
+      <c r="I14" s="60"/>
+      <c r="J14" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="25">
         <v>44889</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="52">
+        <v>24</v>
+      </c>
+      <c r="E15" s="51">
         <v>60</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="61">
+        <v>24</v>
+      </c>
+      <c r="G15" s="60">
         <v>60</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="33" t="s">
-        <v>28</v>
+      <c r="I15" s="60"/>
+      <c r="J15" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="25">
         <v>44889</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="52">
+        <v>24</v>
+      </c>
+      <c r="E16" s="51">
         <v>60</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="61">
+        <v>24</v>
+      </c>
+      <c r="G16" s="60">
         <v>30</v>
       </c>
       <c r="H16" s="23"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="33" t="s">
-        <v>28</v>
+      <c r="I16" s="60"/>
+      <c r="J16" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="25">
         <v>44889</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="52">
+        <v>24</v>
+      </c>
+      <c r="E17" s="51">
         <v>60</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="61"/>
+      <c r="G17" s="60"/>
       <c r="H17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="61">
+        <v>24</v>
+      </c>
+      <c r="I17" s="60">
         <v>60</v>
       </c>
-      <c r="J17" s="32" t="s">
-        <v>27</v>
+      <c r="J17" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="25">
         <v>44889</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="52">
+        <v>24</v>
+      </c>
+      <c r="E18" s="51">
         <v>90</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="61"/>
+      <c r="G18" s="60"/>
       <c r="H18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="61">
+        <v>24</v>
+      </c>
+      <c r="I18" s="60">
         <v>90</v>
       </c>
-      <c r="J18" s="32" t="s">
-        <v>27</v>
+      <c r="J18" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="25">
         <v>44893</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="52"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="61"/>
+      <c r="G19" s="60"/>
       <c r="H19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="61">
+        <v>24</v>
+      </c>
+      <c r="I19" s="60">
         <v>60</v>
       </c>
-      <c r="J19" s="33" t="s">
-        <v>28</v>
+      <c r="J19" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="25">
         <v>44889</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="51">
+        <v>24</v>
+      </c>
+      <c r="E20" s="50">
         <v>90</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="60"/>
+      <c r="G20" s="59"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="34" t="s">
-        <v>29</v>
+      <c r="I20" s="59"/>
+      <c r="J20" s="33" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="25">
         <v>44883</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="52">
+        <v>24</v>
+      </c>
+      <c r="E21" s="51">
         <v>90</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" s="61"/>
+      <c r="G21" s="60"/>
       <c r="H21" s="23"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="33" t="s">
-        <v>28</v>
+      <c r="I21" s="60"/>
+      <c r="J21" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="25">
         <v>44885</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="52">
+        <v>24</v>
+      </c>
+      <c r="E22" s="51">
         <v>180</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="61"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="23"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="32" t="s">
-        <v>27</v>
+      <c r="I22" s="60"/>
+      <c r="J22" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="25">
         <v>44886</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="52">
+        <v>24</v>
+      </c>
+      <c r="E23" s="51">
         <v>90</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="61"/>
+      <c r="G23" s="60"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="32" t="s">
-        <v>27</v>
+      <c r="I23" s="60"/>
+      <c r="J23" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="25">
         <v>44899</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="52">
+        <v>24</v>
+      </c>
+      <c r="E24" s="51">
         <v>60</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="61">
+        <v>24</v>
+      </c>
+      <c r="G24" s="60">
         <v>90</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="61">
+        <v>24</v>
+      </c>
+      <c r="I24" s="60">
         <v>90</v>
       </c>
-      <c r="J24" s="32" t="s">
-        <v>27</v>
+      <c r="J24" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="25">
         <v>44899</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="52">
+        <v>24</v>
+      </c>
+      <c r="E25" s="51">
         <v>30</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="61">
+        <v>24</v>
+      </c>
+      <c r="G25" s="60">
         <v>60</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="61">
+        <v>24</v>
+      </c>
+      <c r="I25" s="60">
         <v>60</v>
       </c>
-      <c r="J25" s="32" t="s">
-        <v>27</v>
+      <c r="J25" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="25">
         <v>44902</v>
       </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="52"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="61">
+        <v>24</v>
+      </c>
+      <c r="G26" s="60">
         <v>240</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="61">
+        <v>24</v>
+      </c>
+      <c r="I26" s="60">
         <v>300</v>
       </c>
-      <c r="J26" s="32" t="s">
-        <v>27</v>
+      <c r="J26" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="28" t="s">
-        <v>49</v>
+      <c r="B27" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="25">
         <v>44902</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="52">
+        <v>24</v>
+      </c>
+      <c r="E27" s="51">
         <v>15</v>
       </c>
       <c r="F27" s="7"/>
-      <c r="G27" s="62"/>
+      <c r="G27" s="61"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="32" t="s">
-        <v>27</v>
+      <c r="I27" s="61"/>
+      <c r="J27" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="28" t="s">
-        <v>40</v>
+      <c r="B28" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="C28" s="25">
         <v>44904</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="52">
+        <v>24</v>
+      </c>
+      <c r="E28" s="51">
         <v>120</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="61">
+        <v>24</v>
+      </c>
+      <c r="G28" s="60">
         <v>180</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="61">
+        <v>24</v>
+      </c>
+      <c r="I28" s="60">
         <v>60</v>
       </c>
-      <c r="J28" s="32" t="s">
-        <v>27</v>
+      <c r="J28" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="25">
         <v>44904</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="52">
+        <v>24</v>
+      </c>
+      <c r="E29" s="51">
         <v>15</v>
       </c>
       <c r="F29" s="7"/>
-      <c r="G29" s="61"/>
+      <c r="G29" s="60"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="32" t="s">
-        <v>27</v>
+      <c r="I29" s="60"/>
+      <c r="J29" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="25">
         <v>44904</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="52">
+        <v>24</v>
+      </c>
+      <c r="E30" s="51">
         <v>90</v>
       </c>
       <c r="F30" s="7"/>
-      <c r="G30" s="61"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="32" t="s">
-        <v>27</v>
+      <c r="I30" s="60"/>
+      <c r="J30" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="31" t="s">
-        <v>43</v>
+      <c r="B31" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="70">
+        <v>21</v>
+      </c>
+      <c r="D31" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="69">
         <v>15</v>
       </c>
-      <c r="F31" s="72"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="32" t="s">
-        <v>27</v>
+      <c r="F31" s="71"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="2:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="B32" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="87">
+      <c r="B32" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="84">
         <v>44915</v>
       </c>
-      <c r="D32" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="53">
+      <c r="D32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="52">
         <v>240</v>
       </c>
-      <c r="F32" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="63">
+      <c r="F32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="62">
         <v>90</v>
       </c>
-      <c r="H32" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="63">
+      <c r="H32" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="62">
         <v>90</v>
       </c>
-      <c r="J32" s="47" t="s">
-        <v>27</v>
+      <c r="J32" s="46" t="s">
+        <v>26</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="87">
+        <v>35</v>
+      </c>
+      <c r="C33" s="84">
         <v>44915</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="54">
+        <v>24</v>
+      </c>
+      <c r="E33" s="53">
         <v>90</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="60"/>
+      <c r="G33" s="59"/>
       <c r="H33" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="60">
+        <v>24</v>
+      </c>
+      <c r="I33" s="59">
         <v>60</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>27</v>
+      <c r="J33" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="87">
+        <v>14</v>
+      </c>
+      <c r="C34" s="84">
         <v>44915</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="52">
+        <v>24</v>
+      </c>
+      <c r="E34" s="51">
         <v>60</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="61">
+        <v>24</v>
+      </c>
+      <c r="G34" s="60">
         <v>60</v>
       </c>
       <c r="H34" s="23"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="33" t="s">
-        <v>28</v>
+      <c r="I34" s="60"/>
+      <c r="J34" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="87">
+        <v>58</v>
+      </c>
+      <c r="C35" s="84">
         <v>44917</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="52"/>
+      <c r="E35" s="51"/>
       <c r="F35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="61">
+        <v>24</v>
+      </c>
+      <c r="G35" s="60">
         <v>90</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="61">
+        <v>24</v>
+      </c>
+      <c r="I35" s="60">
         <v>90</v>
       </c>
-      <c r="J35" s="32" t="s">
-        <v>27</v>
+      <c r="J35" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="87">
+      <c r="B36" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="84">
         <v>44917</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="52"/>
+      <c r="E36" s="51"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="61"/>
+      <c r="G36" s="60"/>
       <c r="H36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="61">
+        <v>24</v>
+      </c>
+      <c r="I36" s="60">
         <v>30</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>27</v>
+      <c r="J36" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="87">
+        <v>44</v>
+      </c>
+      <c r="C37" s="84">
         <v>44917</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="52"/>
+      <c r="E37" s="51"/>
       <c r="F37" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="61">
+        <v>24</v>
+      </c>
+      <c r="G37" s="60">
         <v>60</v>
       </c>
       <c r="H37" s="7"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="33" t="s">
-        <v>28</v>
+      <c r="I37" s="60"/>
+      <c r="J37" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="87">
+        <v>37</v>
+      </c>
+      <c r="C38" s="84">
         <v>44917</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="52"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="61">
+        <v>24</v>
+      </c>
+      <c r="G38" s="60">
         <v>120</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" s="61">
+        <v>24</v>
+      </c>
+      <c r="I38" s="60">
         <v>120</v>
       </c>
-      <c r="J38" s="33" t="s">
-        <v>28</v>
+      <c r="J38" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="25">
         <v>44936</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="52"/>
+      <c r="E39" s="51"/>
       <c r="F39" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="61">
+        <v>24</v>
+      </c>
+      <c r="G39" s="60">
         <v>240</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" s="61">
+        <v>24</v>
+      </c>
+      <c r="I39" s="60">
         <v>240</v>
       </c>
-      <c r="J39" s="32" t="s">
-        <v>27</v>
+      <c r="J39" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="28" t="s">
-        <v>49</v>
+      <c r="B40" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="C40" s="25">
         <v>44936</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="52">
+        <v>24</v>
+      </c>
+      <c r="E40" s="51">
         <v>30</v>
       </c>
       <c r="F40" s="7"/>
-      <c r="G40" s="62"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="7"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="32" t="s">
-        <v>27</v>
+      <c r="I40" s="61"/>
+      <c r="J40" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="86" t="s">
-        <v>50</v>
+      <c r="B41" s="83" t="s">
+        <v>49</v>
       </c>
       <c r="C41" s="25">
         <v>44936</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="52">
+        <v>24</v>
+      </c>
+      <c r="E41" s="51">
         <v>300</v>
       </c>
       <c r="F41" s="7"/>
-      <c r="G41" s="62"/>
+      <c r="G41" s="61"/>
       <c r="H41" s="7"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="32" t="s">
-        <v>27</v>
+      <c r="I41" s="61"/>
+      <c r="J41" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="28" t="s">
-        <v>40</v>
+      <c r="B42" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="C42" s="25">
         <v>44936</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="52">
+        <v>24</v>
+      </c>
+      <c r="E42" s="51">
         <v>60</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="61">
+        <v>24</v>
+      </c>
+      <c r="G42" s="60">
         <v>90</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I42" s="61">
+        <v>24</v>
+      </c>
+      <c r="I42" s="60">
         <v>90</v>
       </c>
-      <c r="J42" s="32" t="s">
-        <v>27</v>
+      <c r="J42" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="25">
         <v>44936</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="52">
+        <v>24</v>
+      </c>
+      <c r="E43" s="51">
         <v>30</v>
       </c>
       <c r="F43" s="7"/>
-      <c r="G43" s="61"/>
+      <c r="G43" s="60"/>
       <c r="H43" s="7"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="32" t="s">
-        <v>27</v>
+      <c r="I43" s="60"/>
+      <c r="J43" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" s="25">
         <v>44936</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="52">
+        <v>24</v>
+      </c>
+      <c r="E44" s="51">
         <v>180</v>
       </c>
       <c r="F44" s="7"/>
-      <c r="G44" s="61"/>
+      <c r="G44" s="60"/>
       <c r="H44" s="7"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="32" t="s">
+      <c r="I44" s="60"/>
+      <c r="J44" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="69"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="73"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="51">
+        <v>30</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="60">
+        <v>120</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="60">
+        <v>120</v>
+      </c>
+      <c r="J46" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="51">
+        <v>60</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="60"/>
+      <c r="H47" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="60"/>
+      <c r="J47" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="51"/>
+      <c r="F48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" s="60"/>
+      <c r="H48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="60"/>
+      <c r="J48" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="51"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="32" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B46" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="52">
-        <v>30</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="61">
-        <v>120</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I46" s="61">
-        <v>120</v>
-      </c>
-      <c r="J46" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B47" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E47" s="52">
-        <v>60</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="61"/>
-      <c r="H47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I47" s="61"/>
-      <c r="J47" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B48" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="52"/>
-      <c r="F48" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="61"/>
-      <c r="H48" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="61"/>
-      <c r="J48" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="52"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="33" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E50" s="52"/>
+      <c r="D50" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="51"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="61"/>
+      <c r="G50" s="60"/>
       <c r="H50" s="23"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="33" t="s">
-        <v>28</v>
+      <c r="I50" s="60"/>
+      <c r="J50" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C51" s="13"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="52"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="51"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="61"/>
+      <c r="G51" s="60"/>
       <c r="H51" s="23"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="33"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="32"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="52"/>
+        <v>24</v>
+      </c>
+      <c r="E52" s="51"/>
       <c r="F52" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G52" s="60"/>
       <c r="H52" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I52" s="61"/>
-      <c r="J52" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I52" s="60"/>
+      <c r="J52" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C53" s="13"/>
-      <c r="D53" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E53" s="52"/>
+      <c r="D53" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="51"/>
       <c r="F53" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G53" s="60"/>
       <c r="H53" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="61"/>
-      <c r="J53" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I53" s="60"/>
+      <c r="J53" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B54" s="68" t="s">
-        <v>79</v>
+      <c r="B54" s="67" t="s">
+        <v>76</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E54" s="52"/>
+        <v>24</v>
+      </c>
+      <c r="E54" s="51"/>
       <c r="F54" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G54" s="60"/>
       <c r="H54" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I54" s="61"/>
-      <c r="J54" s="32"/>
+        <v>24</v>
+      </c>
+      <c r="I54" s="60"/>
+      <c r="J54" s="31"/>
     </row>
     <row r="55" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C55" s="13"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="52"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="51"/>
       <c r="F55" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G55" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G55" s="60"/>
       <c r="H55" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I55" s="61"/>
-      <c r="J55" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I55" s="60"/>
+      <c r="J55" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="52"/>
+      <c r="D56" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="51"/>
       <c r="F56" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G56" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G56" s="60"/>
       <c r="H56" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I56" s="61"/>
-      <c r="J56" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I56" s="60"/>
+      <c r="J56" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="60"/>
+      <c r="H57" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I57" s="60"/>
+      <c r="J57" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="61"/>
-      <c r="H57" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I57" s="61"/>
-      <c r="J57" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="C58" s="13"/>
-      <c r="D58" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E58" s="52"/>
+      <c r="D58" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="51"/>
       <c r="F58" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G58" s="60"/>
       <c r="H58" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I58" s="61"/>
-      <c r="J58" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I58" s="60"/>
+      <c r="J58" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="29" t="s">
-        <v>61</v>
+      <c r="B59" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="C59" s="13"/>
-      <c r="D59" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E59" s="52"/>
+      <c r="D59" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="51"/>
       <c r="F59" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G59" s="60"/>
       <c r="H59" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I59" s="61"/>
-      <c r="J59" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I59" s="60"/>
+      <c r="J59" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="28" t="s">
-        <v>49</v>
+      <c r="B60" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="C60" s="13"/>
-      <c r="D60" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E60" s="52"/>
+      <c r="D60" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="51"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="61"/>
+      <c r="G60" s="60"/>
       <c r="H60" s="23"/>
-      <c r="I60" s="61"/>
-      <c r="J60" s="32" t="s">
-        <v>27</v>
+      <c r="I60" s="60"/>
+      <c r="J60" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C61" s="13"/>
-      <c r="D61" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E61" s="52">
+      <c r="D61" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="51">
         <v>420</v>
       </c>
       <c r="F61" s="9"/>
-      <c r="G61" s="61"/>
+      <c r="G61" s="60"/>
       <c r="H61" s="23"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="32" t="s">
-        <v>27</v>
+      <c r="I61" s="60"/>
+      <c r="J61" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="28" t="s">
-        <v>40</v>
+      <c r="B62" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="C62" s="13"/>
-      <c r="D62" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E62" s="52"/>
+      <c r="D62" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="51"/>
       <c r="F62" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G62" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="G62" s="60"/>
       <c r="H62" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I62" s="61"/>
-      <c r="J62" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I62" s="60"/>
+      <c r="J62" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C63" s="13"/>
-      <c r="D63" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E63" s="52"/>
+      <c r="D63" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="51"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="61"/>
+      <c r="G63" s="60"/>
       <c r="H63" s="23"/>
-      <c r="I63" s="61"/>
-      <c r="J63" s="32" t="s">
-        <v>27</v>
+      <c r="I63" s="60"/>
+      <c r="J63" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" s="52"/>
+      <c r="D64" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="51"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="61"/>
+      <c r="G64" s="60"/>
       <c r="H64" s="23"/>
-      <c r="I64" s="61"/>
-      <c r="J64" s="32" t="s">
-        <v>27</v>
+      <c r="I64" s="60"/>
+      <c r="J64" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="C65" s="14"/>
-      <c r="D65" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E65" s="55"/>
+      <c r="D65" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="54"/>
       <c r="F65" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G65" s="64"/>
+        <v>24</v>
+      </c>
+      <c r="G65" s="63"/>
       <c r="H65" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I65" s="64"/>
-      <c r="J65" s="32" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I65" s="63"/>
+      <c r="J65" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B66" s="44" t="s">
-        <v>55</v>
+      <c r="B66" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="E66" s="70"/>
-      <c r="F66" s="71"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="71"/>
-      <c r="I66" s="70"/>
-      <c r="J66" s="32" t="s">
-        <v>27</v>
+        <v>78</v>
+      </c>
+      <c r="D66" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="69"/>
+      <c r="F66" s="70"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="70"/>
+      <c r="I66" s="69"/>
+      <c r="J66" s="31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C67" s="41"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="78">
+      <c r="C67" s="40"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="77">
         <f>SUM(E4:E66)</f>
         <v>3690</v>
       </c>
-      <c r="F67" s="79"/>
-      <c r="G67" s="78">
+      <c r="F67" s="78"/>
+      <c r="G67" s="77">
         <f>SUM(G4:G66)</f>
         <v>2265</v>
       </c>
-      <c r="H67" s="79"/>
-      <c r="I67" s="78">
+      <c r="H67" s="78"/>
+      <c r="I67" s="77">
         <f>SUM(I4:I66)</f>
         <v>2430</v>
       </c>
-      <c r="J67" s="77" t="s">
-        <v>67</v>
+      <c r="J67" s="76" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C68" s="41"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="78">
+      <c r="C68" s="40"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="77">
         <f>E67/60</f>
         <v>61.5</v>
       </c>
-      <c r="F68" s="79"/>
-      <c r="G68" s="78">
+      <c r="F68" s="78"/>
+      <c r="G68" s="77">
         <f>G67/60</f>
         <v>37.75</v>
       </c>
-      <c r="H68" s="79"/>
-      <c r="I68" s="78">
+      <c r="H68" s="78"/>
+      <c r="I68" s="77">
         <f>I67/60</f>
         <v>40.5</v>
       </c>
-      <c r="J68" s="77" t="s">
-        <v>68</v>
+      <c r="J68" s="76" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B69" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="82">
+      <c r="B69" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="81">
         <v>4200</v>
       </c>
-      <c r="D69" s="82">
+      <c r="D69" s="81">
         <f>C69/60</f>
         <v>70</v>
       </c>
-      <c r="E69" s="80">
+      <c r="E69" s="79">
         <f>E68+D69</f>
         <v>131.5</v>
       </c>
-      <c r="F69" s="81"/>
-      <c r="G69" s="80">
+      <c r="F69" s="80"/>
+      <c r="G69" s="79">
         <f>G68+D69</f>
         <v>107.75</v>
       </c>
-      <c r="H69" s="81"/>
-      <c r="I69" s="80">
+      <c r="H69" s="80"/>
+      <c r="I69" s="79">
         <f>I68+D69</f>
         <v>110.5</v>
       </c>
-      <c r="J69" s="76" t="s">
-        <v>69</v>
+      <c r="J69" s="75" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C70" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70" s="42"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="56"/>
-      <c r="J70" s="43"/>
+      <c r="C70" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="41"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="41"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="42"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C72" s="85"/>
+      <c r="C72"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B73" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C73"/>
-      <c r="E73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="I73" s="58"/>
+      <c r="E73" s="57"/>
+      <c r="G73" s="57"/>
+      <c r="I73" s="57"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B74" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C74"/>
-      <c r="E74" s="58"/>
-      <c r="G74" s="58"/>
-      <c r="I74" s="58"/>
+      <c r="E74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="I74" s="57"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B75" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C75"/>
-      <c r="E75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="I75" s="58"/>
+      <c r="E75" s="57"/>
+      <c r="G75" s="57"/>
+      <c r="I75" s="57"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C76"/>
-      <c r="E76" s="58"/>
-      <c r="G76" s="58"/>
-      <c r="I76" s="58"/>
+      <c r="E76" s="57"/>
+      <c r="G76" s="57"/>
+      <c r="I76" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Hinzufuegen Artefakte Audit 4
</commit_message>
<xml_diff>
--- a/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
+++ b/Artefakte/WS2223_Osaj_Sabetnia_AmirKhanian_Projektplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Documents/EP_Projekt/Alba_EP_Local_Repository/EPWS2223_Osaj_Sabetnia_Amir_Khanian/Artefakte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6903A8-1835-D147-8ECB-564C9415A215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04D605A-DA8D-3240-B3CE-0EDA88974C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="560" windowWidth="25380" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="100">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Gesamt Aufwand in std</t>
   </si>
   <si>
-    <t xml:space="preserve">Design Fiction/ Future System (Figma) </t>
-  </si>
-  <si>
     <t>Bug fixes (+ Dokumentation)</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t>Poster  erstellen</t>
-  </si>
-  <si>
-    <t>Evaluation-Methoden und -Techniken</t>
   </si>
   <si>
     <t>Fazit und Takeaways</t>
@@ -346,10 +340,34 @@
     </r>
   </si>
   <si>
-    <t>Projekt Diskussionen/Meetings (Planung, Besprechungen, Gestaltung, Problemlösungen, etc.)</t>
-  </si>
-  <si>
-    <t>Iterration: Betrachtung und Bewertung Alternativen</t>
+    <t>Projekt-Meetings (Planung, Besprechungen, Gestaltung, Problemlösungen, Recherchen, Iterrationen, Verbesserungen etc.)</t>
+  </si>
+  <si>
+    <t>Betrachtung und Bewertung Alternativen</t>
+  </si>
+  <si>
+    <t>Iterration &amp; Evaluation-Methoden und -Techniken</t>
+  </si>
+  <si>
+    <t>https://www.erenja.de/magazin/energieeffizienzklassen-von-haushaltsgeraeten?utm_source=pinterest&amp;utm_id=pinterest</t>
+  </si>
+  <si>
+    <t>https://wohnglueck.de/artikel/auf-oekostrom-umsteigen-17428?utm_source=pt_wohnglueck&amp;utm_medium=owned_social&amp;utm_campaign=pt_spon&amp;pp=1#51c101f6d5ff988cfb8271d006f325795a9589ba</t>
+  </si>
+  <si>
+    <t>Ökostrom</t>
+  </si>
+  <si>
+    <t>Energieklassen</t>
+  </si>
+  <si>
+    <t>Tipps</t>
+  </si>
+  <si>
+    <t>Messen SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Future User-Interface (Figma) </t>
   </si>
 </sst>
 </file>
@@ -665,7 +683,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -858,9 +876,6 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -892,9 +907,31 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1607,14 +1644,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L90"/>
+  <dimension ref="A2:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" style="15" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
@@ -1626,17 +1664,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
@@ -1774,7 +1812,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>37</v>
@@ -1887,7 +1925,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="24">
         <v>44889</v>
@@ -2644,7 +2682,7 @@
         <v>51</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="69" t="s">
         <v>24</v>
@@ -2660,26 +2698,26 @@
     </row>
     <row r="46" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B46" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="46" t="s">
         <v>24</v>
       </c>
       <c r="E46" s="50">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G46" s="59">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="I46" s="59">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="J46" s="30" t="s">
         <v>26</v>
@@ -2708,84 +2746,86 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>15</v>
+    <row r="48" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="99" t="s">
+        <v>59</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="46" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="50"/>
-      <c r="F48" s="9"/>
+      <c r="F48" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="G48" s="59"/>
-      <c r="H48" s="22"/>
+      <c r="H48" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="I48" s="59"/>
-      <c r="J48" s="31" t="s">
-        <v>27</v>
+      <c r="J48" s="30" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>72</v>
+      <c r="B49" s="100" t="s">
+        <v>91</v>
       </c>
       <c r="C49" s="13"/>
-      <c r="D49" s="46"/>
+      <c r="D49" s="46" t="s">
+        <v>24</v>
+      </c>
       <c r="E49" s="50"/>
-      <c r="F49" s="9"/>
+      <c r="F49" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="G49" s="59"/>
-      <c r="H49" s="22"/>
+      <c r="H49" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="I49" s="59"/>
-      <c r="J49" s="31"/>
+      <c r="J49" s="30" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="50"/>
-      <c r="F50" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="D50" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="50">
+        <v>180</v>
+      </c>
+      <c r="F50" s="9"/>
       <c r="G50" s="59"/>
-      <c r="H50" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="H50" s="22"/>
       <c r="I50" s="59"/>
-      <c r="J50" s="30" t="s">
-        <v>26</v>
+      <c r="J50" s="31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="50"/>
-      <c r="F51" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="59"/>
-      <c r="H51" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="59"/>
-      <c r="J51" s="30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="82" t="s">
-        <v>59</v>
+      <c r="B51" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="101"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="103"/>
+      <c r="F51" s="104"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="106"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="46" t="s">
+      <c r="D52" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="50"/>
@@ -2802,8 +2842,8 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>65</v>
+      <c r="B53" s="80" t="s">
+        <v>64</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="46"/>
@@ -2825,8 +2865,8 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>66</v>
+      <c r="B54" s="80" t="s">
+        <v>65</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="46" t="s">
@@ -2852,8 +2892,8 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="2" t="s">
-        <v>64</v>
+      <c r="B55" s="80" t="s">
+        <v>63</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="46" t="s">
@@ -2879,44 +2919,44 @@
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="102" t="s">
-        <v>78</v>
+      <c r="B56" s="107" t="s">
+        <v>99</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="46" t="s">
         <v>24</v>
       </c>
       <c r="E56" s="50"/>
-      <c r="F56" s="46"/>
+      <c r="F56" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="G56" s="59"/>
-      <c r="H56" s="46"/>
+      <c r="H56" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="I56" s="59"/>
-      <c r="J56" s="30"/>
+      <c r="J56" s="30" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="100" t="s">
-        <v>93</v>
+      <c r="B57" s="108" t="s">
+        <v>76</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="46" t="s">
         <v>24</v>
       </c>
       <c r="E57" s="50"/>
-      <c r="F57" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="F57" s="46"/>
       <c r="G57" s="59"/>
-      <c r="H57" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="H57" s="46"/>
       <c r="I57" s="59"/>
-      <c r="J57" s="30" t="s">
-        <v>26</v>
-      </c>
+      <c r="J57" s="30"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="101" t="s">
-        <v>75</v>
+      <c r="B58" s="100" t="s">
+        <v>92</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="46" t="s">
@@ -2930,8 +2970,8 @@
       <c r="J58" s="30"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="101" t="s">
-        <v>76</v>
+      <c r="B59" s="100" t="s">
+        <v>74</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="46" t="s">
@@ -2951,7 +2991,7 @@
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="100" t="s">
         <v>46</v>
       </c>
       <c r="C60" s="13"/>
@@ -2968,7 +3008,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="100" t="s">
         <v>47</v>
       </c>
       <c r="C61" s="13"/>
@@ -2976,7 +3016,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="50">
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="59"/>
@@ -2987,7 +3027,7 @@
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="100" t="s">
         <v>38</v>
       </c>
       <c r="C62" s="13"/>
@@ -3008,7 +3048,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="100" t="s">
         <v>39</v>
       </c>
       <c r="C63" s="13"/>
@@ -3025,7 +3065,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="100" t="s">
         <v>40</v>
       </c>
       <c r="C64" s="13"/>
@@ -3042,8 +3082,8 @@
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B65" s="3" t="s">
-        <v>74</v>
+      <c r="B65" s="109" t="s">
+        <v>73</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="46" t="s">
@@ -3067,7 +3107,7 @@
         <v>52</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D66" s="66" t="s">
         <v>24</v>
@@ -3086,17 +3126,17 @@
       <c r="D67" s="40"/>
       <c r="E67" s="75">
         <f>SUM(E4:E66)</f>
-        <v>4200</v>
+        <v>4740</v>
       </c>
       <c r="F67" s="76"/>
       <c r="G67" s="75">
         <f>SUM(G4:G66)</f>
-        <v>3855</v>
+        <v>3915</v>
       </c>
       <c r="H67" s="76"/>
       <c r="I67" s="75">
         <f>SUM(I4:I66)</f>
-        <v>4020</v>
+        <v>4080</v>
       </c>
       <c r="J67" s="74" t="s">
         <v>60</v>
@@ -3107,17 +3147,17 @@
       <c r="D68" s="40"/>
       <c r="E68" s="75">
         <f>E67/60</f>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F68" s="76"/>
       <c r="G68" s="75">
         <f>G67/60</f>
-        <v>64.25</v>
+        <v>65.25</v>
       </c>
       <c r="H68" s="76"/>
       <c r="I68" s="75">
         <f>I67/60</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J68" s="74" t="s">
         <v>61</v>
@@ -3125,28 +3165,28 @@
     </row>
     <row r="69" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B69" s="64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C69" s="79">
-        <v>4450</v>
+        <v>7360</v>
       </c>
       <c r="D69" s="79">
         <f>C69/60</f>
-        <v>74.166666666666671</v>
+        <v>122.66666666666667</v>
       </c>
       <c r="E69" s="77">
         <f>E68+D69</f>
-        <v>144.16666666666669</v>
+        <v>201.66666666666669</v>
       </c>
       <c r="F69" s="78"/>
       <c r="G69" s="77">
         <f>G68+D69</f>
-        <v>138.41666666666669</v>
+        <v>187.91666666666669</v>
       </c>
       <c r="H69" s="78"/>
       <c r="I69" s="77">
         <f>I68+D69</f>
-        <v>141.16666666666669</v>
+        <v>190.66666666666669</v>
       </c>
       <c r="J69" s="73" t="s">
         <v>62</v>
@@ -3154,7 +3194,7 @@
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C70" s="65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D70" s="40"/>
       <c r="E70" s="54"/>
@@ -3168,7 +3208,7 @@
       <c r="C72"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="87" t="s">
+      <c r="B73" s="86" t="s">
         <v>33</v>
       </c>
       <c r="C73" s="3"/>
@@ -3177,93 +3217,121 @@
       <c r="I73" s="56"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="83"/>
-      <c r="C74" s="85"/>
+      <c r="B74" s="82"/>
+      <c r="C74" s="84"/>
       <c r="E74" s="56"/>
       <c r="G74" s="56"/>
       <c r="I74" s="56"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B75" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="85"/>
+      <c r="B75" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" s="84"/>
       <c r="E75" s="56"/>
       <c r="G75" s="56"/>
       <c r="I75" s="56"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="85"/>
+      <c r="B76" s="95" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="84"/>
       <c r="E76" s="56"/>
       <c r="G76" s="56"/>
       <c r="I76" s="56"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B77" s="83"/>
-      <c r="C77" s="89"/>
+      <c r="B77" s="82"/>
+      <c r="C77" s="88"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B78" s="90" t="s">
+      <c r="B78" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" s="90"/>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B79" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="96" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B80" s="91"/>
+      <c r="C80" s="90"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B81" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="88"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B82" s="93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="C78" s="91"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B79" s="92" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" s="97" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="92"/>
-      <c r="C80" s="91"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B81" s="93" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B83" s="83"/>
+      <c r="C83" s="94"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B86" s="85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="89"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B82" s="94" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82" s="98" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B83" s="84"/>
-      <c r="C83" s="95"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B86" s="86" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>90</v>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>